<commit_message>
Update on quality attributes
</commit_message>
<xml_diff>
--- a/quality_attributes.xlsx
+++ b/quality_attributes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mahdijaberzadehansari/GitHub/COSETO/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB632261-9297-9B4C-AD6E-4EA1FD69AD37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14C8DF73-C52B-5845-B606-6085BFEA957F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30240" yWindow="-1460" windowWidth="38400" windowHeight="21100" xr2:uid="{6CA35D8A-39DC-BF43-919D-0C2998EB6032}"/>
   </bookViews>
@@ -109,9 +109,6 @@
     <t>the protection from unauthorized access.</t>
   </si>
   <si>
-    <t>{policy,protection,trust,restrictions,secure,authentication}</t>
-  </si>
-  <si>
     <t>the total cost of ownership, which includes the cost to integrate, test and maintain of the software.</t>
   </si>
   <si>
@@ -163,9 +160,6 @@
     <t>{architectural,platform,technology,infrastructure,hardware,platforms,core,frameworks,structure}</t>
   </si>
   <si>
-    <t>{modularity,decoupling,cohesion,robustness,observability,controllability,understandability,verifiability,diagnosability,unit test,test driven,test,examin,evaluate}</t>
-  </si>
-  <si>
     <t>the expected duration a software component takes to complete its tasks, calculated as the weighted average of the execution times of individual components.</t>
   </si>
   <si>
@@ -196,22 +190,28 @@
     <t>capacity to operate, exchange data, and coexist smoothly with other components, versions, or external systems.</t>
   </si>
   <si>
-    <t>{compatible,supporting,modern,older,major,standards,newer,supported,interoperability,coexistence,integration,conformance,alignment}</t>
-  </si>
-  <si>
     <t>{ease of use,understandability,learnability,operable,operability,learnable,understandable,code quality}</t>
   </si>
   <si>
-    <t>{stability,fault tolerance,robustness,workload,tradeoff,bottlenecks,trustworthiness}</t>
-  </si>
-  <si>
-    <t>{type of license,license compliance requirements,commercial,enterprise,licensing,vendor,open-source,proprietary,copyright,copyleft,source‑code disclosure,usage limits,royalty payments}</t>
-  </si>
-  <si>
     <t>{modularity,reuse}</t>
   </si>
   <si>
     <t>{scalable,elasticity,expandability,load‑resilience,capacity}</t>
+  </si>
+  <si>
+    <t>{stability,fault tolerance,robustness,trustworthiness}</t>
+  </si>
+  <si>
+    <t>{type of license,license compliance requirements,licensing,proprietary,copyright,copyleft,usage limits}</t>
+  </si>
+  <si>
+    <t>{modularity,decoupling,cohesion,robustness,observability,controllability,verifiability,diagnosability,unit test,test driven,test,examin,evaluate}</t>
+  </si>
+  <si>
+    <t>{compatible,interoperability,coexistence,integration,conformance,alignment}</t>
+  </si>
+  <si>
+    <t>{authentication,authorization,auth,login}</t>
   </si>
 </sst>
 </file>
@@ -1089,7 +1089,7 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1125,7 +1125,7 @@
         <v>25</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -1153,7 +1153,7 @@
         <v>28</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>29</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -1164,10 +1164,10 @@
         <v>18</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -1178,10 +1178,10 @@
         <v>3</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -1192,10 +1192,10 @@
         <v>15</v>
       </c>
       <c r="C7" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -1206,10 +1206,10 @@
         <v>22</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -1220,10 +1220,10 @@
         <v>23</v>
       </c>
       <c r="C9" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -1234,10 +1234,10 @@
         <v>6</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -1248,10 +1248,10 @@
         <v>13</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -1262,10 +1262,10 @@
         <v>12</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -1276,7 +1276,7 @@
         <v>20</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>21</v>
@@ -1290,10 +1290,10 @@
         <v>7</v>
       </c>
       <c r="C14" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="15" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -1304,10 +1304,10 @@
         <v>4</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>47</v>
+        <v>61</v>
       </c>
     </row>
     <row r="16" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -1318,10 +1318,10 @@
         <v>14</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="17" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -1332,10 +1332,10 @@
         <v>8</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
     </row>
     <row r="18" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -1346,10 +1346,10 @@
         <v>11</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="19" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -1360,10 +1360,10 @@
         <v>19</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
     </row>
     <row r="20" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -1374,10 +1374,10 @@
         <v>17</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="21" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -1388,10 +1388,10 @@
         <v>10</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>